<commit_message>
Add all 17 IT templates (renamed IT_WBS to IT_Project_Plan) and 12 Product templates
</commit_message>
<xml_diff>
--- a/static/templates/IT_RAID_Log.xlsx
+++ b/static/templates/IT_RAID_Log.xlsx
@@ -449,14 +449,14 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>PRODUCT - OPEN ACTION ITEM LOG</t>
+          <t>IT - OPEN ACTION ITEM LOG</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Project: PRODUCT RAID Log</t>
+          <t>Project: IT RAID Log</t>
         </is>
       </c>
     </row>
@@ -737,7 +737,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Security Team</t>
+          <t>Ethics Committee</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -782,7 +782,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>IT Compliance Officers</t>
+          <t>Compliance Officers</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">

</xml_diff>